<commit_message>
It works somehow. Now on to dispersal.
</commit_message>
<xml_diff>
--- a/filoha_lifetable.xlsx
+++ b/filoha_lifetable.xlsx
@@ -380,8 +380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,7 +488,7 @@
         <v>0.05</v>
       </c>
       <c r="C7">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0.05</v>
@@ -506,7 +506,7 @@
         <v>0.05</v>
       </c>
       <c r="C8">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>0.05</v>
@@ -524,7 +524,7 @@
         <v>0.05</v>
       </c>
       <c r="C9">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>0.05</v>
@@ -542,7 +542,7 @@
         <v>0.05</v>
       </c>
       <c r="C10">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0.05</v>
@@ -560,7 +560,7 @@
         <v>0.05</v>
       </c>
       <c r="C11">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>0.05</v>
@@ -578,7 +578,7 @@
         <v>0.05</v>
       </c>
       <c r="C12">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0.05</v>
@@ -596,7 +596,7 @@
         <v>0.05</v>
       </c>
       <c r="C13">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E13">
         <v>0.05</v>
@@ -614,7 +614,7 @@
         <v>0.05</v>
       </c>
       <c r="C14">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E14">
         <v>0.05</v>
@@ -632,7 +632,7 @@
         <v>0.05</v>
       </c>
       <c r="C15">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E15">
         <v>0.05</v>
@@ -647,13 +647,13 @@
         <v>6.5</v>
       </c>
       <c r="B16">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C16">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E16">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -665,13 +665,13 @@
         <v>7</v>
       </c>
       <c r="B17">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C17">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E17">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -683,13 +683,13 @@
         <v>7.5</v>
       </c>
       <c r="B18">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C18">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E18">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -701,13 +701,13 @@
         <v>8</v>
       </c>
       <c r="B19">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C19">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E19">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -719,13 +719,13 @@
         <v>8.5</v>
       </c>
       <c r="B20">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C20">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E20">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -737,13 +737,13 @@
         <v>9</v>
       </c>
       <c r="B21">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C21">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E21">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -755,13 +755,13 @@
         <v>9.5</v>
       </c>
       <c r="B22">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C22">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E22">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -773,13 +773,13 @@
         <v>10</v>
       </c>
       <c r="B23">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C23">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E23">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -791,13 +791,13 @@
         <v>10.5</v>
       </c>
       <c r="B24">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C24">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E24">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -809,13 +809,13 @@
         <v>11</v>
       </c>
       <c r="B25">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C25">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E25">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -827,13 +827,13 @@
         <v>11.5</v>
       </c>
       <c r="B26">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C26">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E26">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -845,13 +845,13 @@
         <v>12</v>
       </c>
       <c r="B27">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C27">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E27">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -863,13 +863,13 @@
         <v>12.5</v>
       </c>
       <c r="B28">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C28">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E28">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -881,13 +881,13 @@
         <v>13</v>
       </c>
       <c r="B29">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C29">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E29">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -899,13 +899,13 @@
         <v>13.5</v>
       </c>
       <c r="B30">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C30">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E30">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -917,13 +917,13 @@
         <v>14</v>
       </c>
       <c r="B31">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C31">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E31">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -935,13 +935,13 @@
         <v>14.5</v>
       </c>
       <c r="B32">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C32">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E32">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -953,13 +953,13 @@
         <v>15</v>
       </c>
       <c r="B33">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C33">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E33">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -971,13 +971,13 @@
         <v>15.5</v>
       </c>
       <c r="B34">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C34">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E34">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -989,13 +989,13 @@
         <v>16</v>
       </c>
       <c r="B35">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C35">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E35">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1007,13 +1007,13 @@
         <v>16.5</v>
       </c>
       <c r="B36">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C36">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E36">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -1025,13 +1025,13 @@
         <v>17</v>
       </c>
       <c r="B37">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C37">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E37">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1043,13 +1043,13 @@
         <v>17.5</v>
       </c>
       <c r="B38">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C38">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E38">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -1061,13 +1061,13 @@
         <v>18</v>
       </c>
       <c r="B39">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C39">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E39">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1079,13 +1079,13 @@
         <v>18.5</v>
       </c>
       <c r="B40">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C40">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E40">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -1097,13 +1097,13 @@
         <v>19</v>
       </c>
       <c r="B41">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C41">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E41">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -1115,13 +1115,13 @@
         <v>19.5</v>
       </c>
       <c r="B42">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C42">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E42">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -1133,13 +1133,13 @@
         <v>20</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F43">
         <v>0</v>

</xml_diff>

<commit_message>
The compability seems to work, picked randomly. Can now be implemented into a challenge function.
</commit_message>
<xml_diff>
--- a/filoha_lifetable.xlsx
+++ b/filoha_lifetable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="23256" windowHeight="12588"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="23256" windowHeight="12588" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>FEMALE</t>
   </si>
@@ -34,6 +34,21 @@
   </si>
   <si>
     <t>qx</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Type 1 high round</t>
+  </si>
+  <si>
+    <t>Type 2 low round</t>
+  </si>
+  <si>
+    <t>Type 3  high peak</t>
+  </si>
+  <si>
+    <t>Type 4 low peak</t>
   </si>
 </sst>
 </file>
@@ -380,7 +395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16:E43"/>
     </sheetView>
   </sheetViews>
@@ -1160,12 +1175,863 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f xml:space="preserve"> A3 + 0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" ref="A5:A45" si="0" xml:space="preserve"> A4 + 0.5</f>
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <f>B15/2</f>
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <f>D15/2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="B16">
+        <v>48</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:C43" si="1">B16/2</f>
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ref="E16:E43" si="2">D16/2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>61</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>30.5</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="B18">
+        <v>65</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>32.5</v>
+      </c>
+      <c r="D18">
+        <v>9</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>68</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="D19">
+        <v>12</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+      <c r="B20">
+        <v>71</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>35.5</v>
+      </c>
+      <c r="D20">
+        <v>16</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>73</v>
+      </c>
+      <c r="C21">
+        <f>B21/2</f>
+        <v>36.5</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+      <c r="B22">
+        <v>75</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>37.5</v>
+      </c>
+      <c r="D22">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>76</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="D23">
+        <v>30</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>10.5</v>
+      </c>
+      <c r="B24">
+        <v>77</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>38.5</v>
+      </c>
+      <c r="D24">
+        <v>40</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B25">
+        <v>78</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="D25">
+        <v>50</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
+      <c r="B26">
+        <v>79</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>39.5</v>
+      </c>
+      <c r="D26">
+        <v>60</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>79.5</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>39.75</v>
+      </c>
+      <c r="D27">
+        <v>75</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+      <c r="B28">
+        <v>80</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="D28">
+        <v>90</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B29">
+        <v>80</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="D29">
+        <v>96</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>13.5</v>
+      </c>
+      <c r="B30">
+        <v>80</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="D30">
+        <v>100</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B31">
+        <v>79.5</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>39.75</v>
+      </c>
+      <c r="D31">
+        <v>96</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>14.5</v>
+      </c>
+      <c r="B32">
+        <v>79</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>39.5</v>
+      </c>
+      <c r="D32">
+        <v>90</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B33">
+        <v>78</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="D33">
+        <v>75</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>15.5</v>
+      </c>
+      <c r="B34">
+        <v>77</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>38.5</v>
+      </c>
+      <c r="D34">
+        <v>60</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B35">
+        <v>76</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="D35">
+        <v>50</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>16.5</v>
+      </c>
+      <c r="B36">
+        <v>75</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>37.5</v>
+      </c>
+      <c r="D36">
+        <v>40</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B37">
+        <v>73</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>36.5</v>
+      </c>
+      <c r="D37">
+        <v>30</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+      <c r="B38">
+        <v>71</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>35.5</v>
+      </c>
+      <c r="D38">
+        <v>22</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B39">
+        <v>68</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="D39">
+        <v>16</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>18.5</v>
+      </c>
+      <c r="B40">
+        <v>65</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="1"/>
+        <v>32.5</v>
+      </c>
+      <c r="D40">
+        <v>11</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B41">
+        <v>61</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="1"/>
+        <v>30.5</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <f xml:space="preserve"> A41 + 0.5</f>
+        <v>19.5</v>
+      </c>
+      <c r="B42">
+        <v>48</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="D42">
+        <v>4</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B43">
+        <v>30</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <f xml:space="preserve"> A43 + 0.5</f>
+        <v>20.5</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Dispersal/death seems to work EXCEPT for moving females to a new group when taken over from outside natal group
</commit_message>
<xml_diff>
--- a/filoha_lifetable.xlsx
+++ b/filoha_lifetable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="23256" windowHeight="12588" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="11532" windowHeight="7656"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,6 +104,1265 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$3:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$3:$B$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>79.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>79.5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$3:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$3:$C$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>35.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>36.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>38.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>39.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>39.75</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>39.75</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>39.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>38.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>36.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$3:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$3:$D$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$3:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$3:$E$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="195400832"/>
+        <c:axId val="195186048"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="195400832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="195186048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="195186048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="195400832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -395,7 +1654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16:E43"/>
     </sheetView>
   </sheetViews>
@@ -1177,8 +2436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2033,6 +3292,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
save data is broken
</commit_message>
<xml_diff>
--- a/filoha_lifetable.xlsx
+++ b/filoha_lifetable.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -1278,11 +1278,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="195400832"/>
-        <c:axId val="195186048"/>
+        <c:axId val="213905408"/>
+        <c:axId val="213906944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="195400832"/>
+        <c:axId val="213905408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1292,12 +1292,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195186048"/>
+        <c:crossAx val="213906944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="195186048"/>
+        <c:axId val="213906944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1308,14 +1308,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195400832"/>
+        <c:crossAx val="213905408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1654,8 +1653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16:E43"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1705,13 +1704,13 @@
         <v>0.5</v>
       </c>
       <c r="B4">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1870,7 +1869,7 @@
         <v>0.05</v>
       </c>
       <c r="C13">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E13">
         <v>0.05</v>
@@ -1888,7 +1887,7 @@
         <v>0.05</v>
       </c>
       <c r="C14">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E14">
         <v>0.05</v>
@@ -1906,7 +1905,7 @@
         <v>0.05</v>
       </c>
       <c r="C15">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E15">
         <v>0.05</v>
@@ -1921,13 +1920,13 @@
         <v>6.5</v>
       </c>
       <c r="B16">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C16">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E16">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1939,13 +1938,13 @@
         <v>7</v>
       </c>
       <c r="B17">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C17">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E17">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1957,13 +1956,13 @@
         <v>7.5</v>
       </c>
       <c r="B18">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C18">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E18">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1975,103 +1974,103 @@
         <v>8</v>
       </c>
       <c r="B19">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C19">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E19">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="B20">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C20">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E20">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B21">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C21">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E21">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
       <c r="B22">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C22">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E22">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B23">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C23">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E23">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>10.5</v>
       </c>
       <c r="B24">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C24">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E24">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -2083,13 +2082,13 @@
         <v>11</v>
       </c>
       <c r="B25">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C25">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E25">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -2101,13 +2100,13 @@
         <v>11.5</v>
       </c>
       <c r="B26">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C26">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E26">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -2119,13 +2118,13 @@
         <v>12</v>
       </c>
       <c r="B27">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C27">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E27">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -2137,13 +2136,13 @@
         <v>12.5</v>
       </c>
       <c r="B28">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C28">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E28">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -2155,13 +2154,13 @@
         <v>13</v>
       </c>
       <c r="B29">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C29">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E29">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -2173,13 +2172,13 @@
         <v>13.5</v>
       </c>
       <c r="B30">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C30">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E30">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -2191,13 +2190,13 @@
         <v>14</v>
       </c>
       <c r="B31">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C31">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E31">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -2209,13 +2208,13 @@
         <v>14.5</v>
       </c>
       <c r="B32">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C32">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E32">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -2227,13 +2226,13 @@
         <v>15</v>
       </c>
       <c r="B33">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C33">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E33">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -2245,13 +2244,13 @@
         <v>15.5</v>
       </c>
       <c r="B34">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C34">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E34">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -2263,13 +2262,13 @@
         <v>16</v>
       </c>
       <c r="B35">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C35">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E35">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -2281,13 +2280,13 @@
         <v>16.5</v>
       </c>
       <c r="B36">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C36">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E36">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -2299,13 +2298,13 @@
         <v>17</v>
       </c>
       <c r="B37">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C37">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E37">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -2317,13 +2316,13 @@
         <v>17.5</v>
       </c>
       <c r="B38">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C38">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E38">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -2335,13 +2334,13 @@
         <v>18</v>
       </c>
       <c r="B39">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C39">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E39">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -2353,13 +2352,13 @@
         <v>18.5</v>
       </c>
       <c r="B40">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C40">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E40">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -2371,13 +2370,13 @@
         <v>19</v>
       </c>
       <c r="B41">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C41">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E41">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -2389,10 +2388,10 @@
         <v>19.5</v>
       </c>
       <c r="B42">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C42">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="E42">
         <v>0.1</v>
@@ -2407,13 +2406,13 @@
         <v>20</v>
       </c>
       <c r="B43">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="E43">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F43">
         <v>0</v>

</xml_diff>

<commit_message>
print causes of death at the end of a simulation. Also changed lifetable
</commit_message>
<xml_diff>
--- a/filoha_lifetable.xlsx
+++ b/filoha_lifetable.xlsx
@@ -1278,11 +1278,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="213905408"/>
-        <c:axId val="213906944"/>
+        <c:axId val="253012608"/>
+        <c:axId val="19845888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="213905408"/>
+        <c:axId val="253012608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1292,12 +1292,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213906944"/>
+        <c:crossAx val="19845888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="213906944"/>
+        <c:axId val="19845888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1308,7 +1308,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213905408"/>
+        <c:crossAx val="253012608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1653,8 +1653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1722,13 +1722,13 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1740,13 +1740,13 @@
         <v>1.5</v>
       </c>
       <c r="B6">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1758,13 +1758,13 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1776,13 +1776,13 @@
         <v>2.5</v>
       </c>
       <c r="B8">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1794,13 +1794,13 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1812,13 +1812,13 @@
         <v>3.5</v>
       </c>
       <c r="B10">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1830,13 +1830,13 @@
         <v>4</v>
       </c>
       <c r="B11">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1848,13 +1848,13 @@
         <v>4.5</v>
       </c>
       <c r="B12">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1866,13 +1866,13 @@
         <v>5</v>
       </c>
       <c r="B13">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="C13">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E13">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1884,13 +1884,13 @@
         <v>5.5</v>
       </c>
       <c r="B14">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="C14">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E14">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1902,13 +1902,13 @@
         <v>6</v>
       </c>
       <c r="B15">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="C15">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E15">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1923,10 +1923,10 @@
         <v>0.02</v>
       </c>
       <c r="C16">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E16">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1941,10 +1941,10 @@
         <v>0.02</v>
       </c>
       <c r="C17">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E17">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1959,10 +1959,10 @@
         <v>0.02</v>
       </c>
       <c r="C18">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E18">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1977,10 +1977,10 @@
         <v>0.02</v>
       </c>
       <c r="C19">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E19">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1995,10 +1995,10 @@
         <v>0.02</v>
       </c>
       <c r="C20">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E20">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -2013,10 +2013,10 @@
         <v>0.02</v>
       </c>
       <c r="C21">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E21">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -2031,10 +2031,10 @@
         <v>0.02</v>
       </c>
       <c r="C22">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E22">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -2049,10 +2049,10 @@
         <v>0.02</v>
       </c>
       <c r="C23">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E23">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -2067,10 +2067,10 @@
         <v>0.02</v>
       </c>
       <c r="C24">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E24">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -2085,10 +2085,10 @@
         <v>0.02</v>
       </c>
       <c r="C25">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E25">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -2103,10 +2103,10 @@
         <v>0.02</v>
       </c>
       <c r="C26">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E26">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -2121,10 +2121,10 @@
         <v>0.02</v>
       </c>
       <c r="C27">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E27">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -2139,10 +2139,10 @@
         <v>0.02</v>
       </c>
       <c r="C28">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E28">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -2157,10 +2157,10 @@
         <v>0.02</v>
       </c>
       <c r="C29">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E29">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -2175,10 +2175,10 @@
         <v>0.02</v>
       </c>
       <c r="C30">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E30">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -2193,10 +2193,10 @@
         <v>0.02</v>
       </c>
       <c r="C31">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E31">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -2211,10 +2211,10 @@
         <v>0.02</v>
       </c>
       <c r="C32">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E32">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -2229,10 +2229,10 @@
         <v>0.02</v>
       </c>
       <c r="C33">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E33">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -2247,10 +2247,10 @@
         <v>0.02</v>
       </c>
       <c r="C34">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E34">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -2265,10 +2265,10 @@
         <v>0.02</v>
       </c>
       <c r="C35">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E35">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -2283,10 +2283,10 @@
         <v>0.02</v>
       </c>
       <c r="C36">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E36">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -2301,10 +2301,10 @@
         <v>0.02</v>
       </c>
       <c r="C37">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E37">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -2319,10 +2319,10 @@
         <v>0.02</v>
       </c>
       <c r="C38">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E38">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -2337,10 +2337,10 @@
         <v>0.02</v>
       </c>
       <c r="C39">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E39">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -2355,10 +2355,10 @@
         <v>0.02</v>
       </c>
       <c r="C40">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E40">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -2373,10 +2373,10 @@
         <v>0.02</v>
       </c>
       <c r="C41">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E41">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -2391,10 +2391,10 @@
         <v>0.02</v>
       </c>
       <c r="C42">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E42">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -2419,6 +2419,9 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>0</v>
+      </c>
       <c r="C44">
         <v>0</v>
       </c>
@@ -2436,7 +2439,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E45"/>
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>